<commit_message>
SOECENT-239 | update 1925 Board of Trustees timeline item
</commit_message>
<xml_diff>
--- a/scripts/files/updated_timeline-backup.xlsx
+++ b/scripts/files/updated_timeline-backup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccahong/programming/soe-centennial-nextjs/scripts/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2767DD33-8627-9D44-8F15-F378B91080F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F5D2E2-3AC7-8B4F-B72C-36C8CB5F360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="613">
   <si>
     <t>year</t>
   </si>
@@ -2492,12 +2492,15 @@
   <si>
     <t>Mechanical Engineering student, 1970. | Stanford News Service.</t>
   </si>
+  <si>
+    <t>https://res.cloudinary.com/dsqi5touf/image/upload/v1745510541/20220301_Campus_N6A9748_s9y4su.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2581,6 +2584,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2617,10 +2627,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2667,8 +2678,12 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2888,8 +2903,8 @@
   <dimension ref="A1:E978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2930,8 +2945,8 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>7</v>
+      <c r="E2" s="16" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7964,154 +7979,154 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="E26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="E29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="E31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="E32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="E33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="E34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="E35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="E36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="E37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="E38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="E39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="E40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="E41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="E42" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="E43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="E44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="E45" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="E46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="E47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="E48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="E49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="E50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="E51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="E52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="E53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="E54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="E55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="E56" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="E57" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="E58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="E59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="E60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="E61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="E62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="E63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="E64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="E65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="E66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="E67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="E68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="E69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="E70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="E72" r:id="rId68" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="E73" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="E74" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="E75" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="E76" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="E77" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="E78" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="E79" r:id="rId75" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="E80" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="E81" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="E82" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="E83" r:id="rId79" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="E84" r:id="rId80" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="E85" r:id="rId81" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="E86" r:id="rId82" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="E87" r:id="rId83" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="E88" r:id="rId84" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="E89" r:id="rId85" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="E90" r:id="rId86" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="E91" r:id="rId87" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="E92" r:id="rId88" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="E93" r:id="rId89" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="E94" r:id="rId90" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="E95" r:id="rId91" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="E96" r:id="rId92" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="E97" r:id="rId93" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="E98" r:id="rId94" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="E99" r:id="rId95" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="E100" r:id="rId96" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="E101" r:id="rId97" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="E102" r:id="rId98" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="E103" r:id="rId99" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="E104" r:id="rId100" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="E105" r:id="rId101" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="E106" r:id="rId102" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="E107" r:id="rId103" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="E108" r:id="rId104" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="E109" r:id="rId105" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="E110" r:id="rId106" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="E111" r:id="rId107" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="E112" r:id="rId108" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="E113" r:id="rId109" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="E114" r:id="rId110" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="E115" r:id="rId111" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="E116" r:id="rId112" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="E117" r:id="rId113" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="E118" r:id="rId114" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="E119" r:id="rId115" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="E120" r:id="rId116" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="E121" r:id="rId117" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="E122" r:id="rId118" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="E123" r:id="rId119" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="E124" r:id="rId120" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="E125" r:id="rId121" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="E126" r:id="rId122" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="E127" r:id="rId123" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="E128" r:id="rId124" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="E129" r:id="rId125" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="E130" r:id="rId126" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="E131" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="E132" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="E133" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="E134" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="E135" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="E136" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="E137" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="E138" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="E139" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="E140" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="E141" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="E142" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="E143" r:id="rId139" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="E144" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="E145" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="E146" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="E147" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="E148" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="E149" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="E150" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="E151" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="E152" r:id="rId148" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="E35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="E36" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="E37" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E38" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="E39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="E40" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="E41" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="E42" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="E43" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="E44" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="E45" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="E46" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E47" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="E48" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E49" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E50" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E51" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="E52" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="E53" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="E54" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="E55" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="E56" r:id="rId52" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="E57" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="E58" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="E59" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="E60" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="E61" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="E62" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="E63" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="E64" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="E65" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="E66" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="E67" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="E68" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="E69" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="E70" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="E72" r:id="rId67" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="E73" r:id="rId68" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="E74" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="E75" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="E76" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="E77" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="E78" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="E79" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="E80" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="E81" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="E82" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="E83" r:id="rId78" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="E84" r:id="rId79" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="E85" r:id="rId80" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="E86" r:id="rId81" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="E87" r:id="rId82" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="E88" r:id="rId83" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="E89" r:id="rId84" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="E90" r:id="rId85" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="E91" r:id="rId86" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="E92" r:id="rId87" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="E93" r:id="rId88" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="E94" r:id="rId89" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="E95" r:id="rId90" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="E96" r:id="rId91" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="E97" r:id="rId92" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="E98" r:id="rId93" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="E99" r:id="rId94" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="E100" r:id="rId95" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="E101" r:id="rId96" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="E102" r:id="rId97" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="E103" r:id="rId98" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="E104" r:id="rId99" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="E105" r:id="rId100" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="E106" r:id="rId101" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="E107" r:id="rId102" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="E108" r:id="rId103" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="E109" r:id="rId104" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="E110" r:id="rId105" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="E111" r:id="rId106" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="E112" r:id="rId107" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="E113" r:id="rId108" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="E114" r:id="rId109" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="E115" r:id="rId110" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="E116" r:id="rId111" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="E117" r:id="rId112" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="E118" r:id="rId113" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="E119" r:id="rId114" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="E120" r:id="rId115" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="E121" r:id="rId116" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="E122" r:id="rId117" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="E123" r:id="rId118" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="E124" r:id="rId119" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="E125" r:id="rId120" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="E126" r:id="rId121" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="E127" r:id="rId122" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="E128" r:id="rId123" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="E129" r:id="rId124" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="E130" r:id="rId125" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="E131" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="E132" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="E133" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="E134" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="E135" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="E136" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="E137" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="E138" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="E139" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="E140" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="E141" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="E142" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="E143" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="E144" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="E145" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="E146" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="E147" r:id="rId142" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="E148" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="E149" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="E150" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="E151" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="E152" r:id="rId147" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="E2" r:id="rId148" xr:uid="{744F8530-9FAA-B44D-8212-28FDBD867085}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SOECENT-239 | update 1925 Board of Trustees timeline item (#52)
</commit_message>
<xml_diff>
--- a/scripts/files/updated_timeline-backup.xlsx
+++ b/scripts/files/updated_timeline-backup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccahong/programming/soe-centennial-nextjs/scripts/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2767DD33-8627-9D44-8F15-F378B91080F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F5D2E2-3AC7-8B4F-B72C-36C8CB5F360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="613">
   <si>
     <t>year</t>
   </si>
@@ -2492,12 +2492,15 @@
   <si>
     <t>Mechanical Engineering student, 1970. | Stanford News Service.</t>
   </si>
+  <si>
+    <t>https://res.cloudinary.com/dsqi5touf/image/upload/v1745510541/20220301_Campus_N6A9748_s9y4su.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2581,6 +2584,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2617,10 +2627,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2667,8 +2678,12 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2888,8 +2903,8 @@
   <dimension ref="A1:E978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2930,8 +2945,8 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>7</v>
+      <c r="E2" s="16" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7964,154 +7979,154 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="E26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="E29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="E31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="E32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="E33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="E34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="E35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="E36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="E37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="E38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="E39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="E40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="E41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="E42" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="E43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="E44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="E45" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="E46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="E47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="E48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="E49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="E50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="E51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="E52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="E53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="E54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="E55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="E56" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="E57" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="E58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="E59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="E60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="E61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="E62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="E63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="E64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="E65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="E66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="E67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="E68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="E69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="E70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="E72" r:id="rId68" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="E73" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="E74" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="E75" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="E76" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="E77" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="E78" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="E79" r:id="rId75" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="E80" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="E81" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="E82" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="E83" r:id="rId79" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="E84" r:id="rId80" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="E85" r:id="rId81" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="E86" r:id="rId82" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="E87" r:id="rId83" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="E88" r:id="rId84" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="E89" r:id="rId85" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="E90" r:id="rId86" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="E91" r:id="rId87" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="E92" r:id="rId88" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="E93" r:id="rId89" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="E94" r:id="rId90" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="E95" r:id="rId91" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="E96" r:id="rId92" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="E97" r:id="rId93" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="E98" r:id="rId94" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="E99" r:id="rId95" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="E100" r:id="rId96" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="E101" r:id="rId97" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="E102" r:id="rId98" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="E103" r:id="rId99" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="E104" r:id="rId100" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="E105" r:id="rId101" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="E106" r:id="rId102" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="E107" r:id="rId103" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="E108" r:id="rId104" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="E109" r:id="rId105" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="E110" r:id="rId106" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="E111" r:id="rId107" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="E112" r:id="rId108" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="E113" r:id="rId109" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="E114" r:id="rId110" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="E115" r:id="rId111" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="E116" r:id="rId112" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="E117" r:id="rId113" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="E118" r:id="rId114" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="E119" r:id="rId115" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="E120" r:id="rId116" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="E121" r:id="rId117" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="E122" r:id="rId118" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="E123" r:id="rId119" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="E124" r:id="rId120" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="E125" r:id="rId121" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="E126" r:id="rId122" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="E127" r:id="rId123" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="E128" r:id="rId124" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="E129" r:id="rId125" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="E130" r:id="rId126" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="E131" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="E132" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="E133" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="E134" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="E135" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="E136" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="E137" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="E138" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="E139" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="E140" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="E141" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="E142" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="E143" r:id="rId139" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="E144" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="E145" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="E146" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="E147" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="E148" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="E149" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="E150" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="E151" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="E152" r:id="rId148" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="E35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="E36" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="E37" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E38" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="E39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="E40" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="E41" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="E42" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="E43" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="E44" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="E45" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="E46" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E47" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="E48" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E49" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E50" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E51" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="E52" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="E53" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="E54" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="E55" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="E56" r:id="rId52" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="E57" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="E58" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="E59" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="E60" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="E61" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="E62" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="E63" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="E64" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="E65" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="E66" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="E67" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="E68" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="E69" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="E70" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="E72" r:id="rId67" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="E73" r:id="rId68" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="E74" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="E75" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="E76" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="E77" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="E78" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="E79" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="E80" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="E81" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="E82" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="E83" r:id="rId78" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="E84" r:id="rId79" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="E85" r:id="rId80" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="E86" r:id="rId81" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="E87" r:id="rId82" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="E88" r:id="rId83" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="E89" r:id="rId84" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="E90" r:id="rId85" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="E91" r:id="rId86" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="E92" r:id="rId87" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="E93" r:id="rId88" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="E94" r:id="rId89" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="E95" r:id="rId90" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="E96" r:id="rId91" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="E97" r:id="rId92" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="E98" r:id="rId93" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="E99" r:id="rId94" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="E100" r:id="rId95" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="E101" r:id="rId96" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="E102" r:id="rId97" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="E103" r:id="rId98" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="E104" r:id="rId99" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="E105" r:id="rId100" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="E106" r:id="rId101" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="E107" r:id="rId102" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="E108" r:id="rId103" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="E109" r:id="rId104" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="E110" r:id="rId105" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="E111" r:id="rId106" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="E112" r:id="rId107" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="E113" r:id="rId108" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="E114" r:id="rId109" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="E115" r:id="rId110" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="E116" r:id="rId111" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="E117" r:id="rId112" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="E118" r:id="rId113" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="E119" r:id="rId114" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="E120" r:id="rId115" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="E121" r:id="rId116" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="E122" r:id="rId117" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="E123" r:id="rId118" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="E124" r:id="rId119" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="E125" r:id="rId120" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="E126" r:id="rId121" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="E127" r:id="rId122" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="E128" r:id="rId123" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="E129" r:id="rId124" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="E130" r:id="rId125" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="E131" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="E132" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="E133" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="E134" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="E135" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="E136" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="E137" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="E138" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="E139" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="E140" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="E141" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="E142" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="E143" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="E144" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="E145" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="E146" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="E147" r:id="rId142" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="E148" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="E149" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="E150" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="E151" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="E152" r:id="rId147" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="E2" r:id="rId148" xr:uid="{744F8530-9FAA-B44D-8212-28FDBD867085}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>